<commit_message>
Added excel Clients.xlsx file
</commit_message>
<xml_diff>
--- a/src/main/java/eshop/Clients.xlsx
+++ b/src/main/java/eshop/Clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC5C14C-AAD5-4244-A194-A950091FBAD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E46C2E-31AD-4C9D-A308-C6B997550A00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Snow</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -355,47 +358,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ExcelReader methods created; Initial Tests set up
</commit_message>
<xml_diff>
--- a/src/main/java/eshop/Clients.xlsx
+++ b/src/main/java/eshop/Clients.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E46C2E-31AD-4C9D-A308-C6B997550A00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F9DCAE-7048-4EB7-978A-4463BB2FA71F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +41,24 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>Debby</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Blackmore</t>
   </si>
 </sst>
 </file>
@@ -358,17 +376,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:XFD1048576"/>
+      <selection activeCell="C9" sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="2.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
@@ -415,6 +433,46 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>3423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>